<commit_message>
Se realizó la función para generar el WebController
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelso\Documents\GitHub\proyecto-grado\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA64342B-1CA1-49FB-A82E-B06A3FFB53A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA0052A-38D0-4B85-B42D-EA5BE4D7D1DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,7 +940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -970,6 +972,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -1147,15 +1158,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1163,6 +1165,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1176,14 +1186,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
modificación caso 2 grafo
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="495" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="1095" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="62">
   <si>
     <t>Class</t>
   </si>
@@ -34,18 +34,12 @@
     <t>calls</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.model.BaseEntity</t>
-  </si>
-  <si>
     <t>BaseEntity</t>
   </si>
   <si>
     <t>pet</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.model.Person</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -61,36 +55,21 @@
     <t>owner.org.springframework.samples.petclinic.model.Person</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.owner.Owner</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.owner.Pet</t>
-  </si>
-  <si>
     <t>Pet</t>
   </si>
   <si>
     <t>PetController</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.owner.PetRepository</t>
-  </si>
-  <si>
     <t>PetRepository</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.owner.PetType</t>
-  </si>
-  <si>
     <t>PetType</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.visit.Visit</t>
-  </si>
-  <si>
     <t>Visit</t>
   </si>
   <si>
@@ -139,10 +118,94 @@
     <t>NamedEntity</t>
   </si>
   <si>
-    <t>pet.org.springframework.samples.petclinic.model.NamedEntity</t>
-  </si>
-  <si>
-    <t>UsesClass</t>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Uses Class</t>
+  </si>
+  <si>
+    <t>Has Method</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>pet1</t>
+  </si>
+  <si>
+    <t>PetController.processCreationForm(@PathVariable("ownerId") int ownerId, @RequestBody Pet pet)</t>
+  </si>
+  <si>
+    <t>PetController.processUpdateForm(@PathVariable("ownerId") int ownerId, @PathVariable("petId") int petId, @RequestBody Pet pet)</t>
+  </si>
+  <si>
+    <t>PetController.processFindForm(@PathVariable("ownerId") int ownerId)</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processCreationForm(@PathVariable("ownerId") int ownerId, @RequestBody Pet pet)</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processUpdateForm(@PathVariable("ownerId") int ownerId, @PathVariable("petId") int petId, @RequestBody Pet pet)</t>
+  </si>
+  <si>
+    <t>pet2</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetController.processFindForm(@PathVariable("ownerId") int ownerId)</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.model.BaseEntity</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.model.NamedEntity</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.model.Person</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.Owner</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.Pet</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetController</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetRepository</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetType</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.visit.Visit</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.Owner</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.Pet</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetRepository</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetType</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.visit.Visit</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.model.BaseEntity</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.model.NamedEntity</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.model.Person</t>
   </si>
 </sst>
 </file>
@@ -495,17 +558,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31" customWidth="1"/>
+    <col min="1" max="1" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
@@ -514,324 +578,324 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,91 +903,367 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -934,15 +1274,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.85546875" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
@@ -958,133 +1298,245 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1103,12 +1555,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -1286,6 +1732,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
   <ds:schemaRefs>
@@ -1295,22 +1747,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1326,4 +1762,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Validación para agregar metodos
Se agrego la función para agregar metodos.
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1095" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="3495" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="69">
   <si>
     <t>Class</t>
   </si>
@@ -37,9 +37,6 @@
     <t>BaseEntity</t>
   </si>
   <si>
-    <t>pet</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -133,27 +130,9 @@
     <t>pet1</t>
   </si>
   <si>
-    <t>PetController.processCreationForm(@PathVariable("ownerId") int ownerId, @RequestBody Pet pet)</t>
-  </si>
-  <si>
-    <t>PetController.processUpdateForm(@PathVariable("ownerId") int ownerId, @PathVariable("petId") int petId, @RequestBody Pet pet)</t>
-  </si>
-  <si>
-    <t>PetController.processFindForm(@PathVariable("ownerId") int ownerId)</t>
-  </si>
-  <si>
-    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processCreationForm(@PathVariable("ownerId") int ownerId, @RequestBody Pet pet)</t>
-  </si>
-  <si>
-    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processUpdateForm(@PathVariable("ownerId") int ownerId, @PathVariable("petId") int petId, @RequestBody Pet pet)</t>
-  </si>
-  <si>
     <t>pet2</t>
   </si>
   <si>
-    <t>pet2.org.springframework.samples.petclinic.owner.PetController.processFindForm(@PathVariable("ownerId") int ownerId)</t>
-  </si>
-  <si>
     <t>pet1.org.springframework.samples.petclinic.model.BaseEntity</t>
   </si>
   <si>
@@ -206,6 +185,48 @@
   </si>
   <si>
     <t>pet2.org.springframework.samples.petclinic.model.Person</t>
+  </si>
+  <si>
+    <t>PetController.processCreationForm(int, Pet)</t>
+  </si>
+  <si>
+    <t>PetController.processUpdateForm(int , int , Pet)</t>
+  </si>
+  <si>
+    <t>PetController.processFindForm(int)</t>
+  </si>
+  <si>
+    <t>OwnerController.processCreationForm(Owner)</t>
+  </si>
+  <si>
+    <t>OwnerController.processUpdateOwnerForm(Owner, int)</t>
+  </si>
+  <si>
+    <t>OwnerController.showOwner(int)</t>
+  </si>
+  <si>
+    <t>OwnerController.processFindForm(Owner)</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.samples.petclinic.owner.OwnerController.processUpdateOwnerForm(Owner, int)</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.samples.petclinic.owner.OwnerController.processCreationForm(Owner)</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.samples.petclinic.owner.OwnerController.processFindForm(Owner)</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.samples.petclinic.owner.OwnerController.showOwner(int)</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processUpdateForm(int, int, Pet)</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.processCreationForm(int, Pet)</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetController.processFindForm(int)</t>
   </si>
 </sst>
 </file>
@@ -558,18 +579,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96.140625" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
@@ -578,324 +599,324 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -903,367 +924,459 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
         <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
         <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1274,16 +1387,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+    <col min="2" max="2" width="169.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1298,245 +1411,301 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1546,6 +1715,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1554,7 +1729,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -1732,13 +1907,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1746,7 +1931,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1762,20 +1947,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se agrego la particion de atributos
eso implica los constructores
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelso\Documents\GitHub\proyecto-grado\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8625D-0232-4C4B-90B1-88C45A56FC17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F7CDAF-34F9-4F51-B87A-CAB4EE9EA8C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,23 @@
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Edges" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="84">
   <si>
     <t>Class</t>
   </si>
@@ -249,6 +260,30 @@
   </si>
   <si>
     <t>SpringBootApplication</t>
+  </si>
+  <si>
+    <t>Has field</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.samples.petclinic.owner.PetController.pets</t>
+  </si>
+  <si>
+    <t>PetController.pets</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.pets</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.samples.petclinic.owner.PetController.owners</t>
+  </si>
+  <si>
+    <t>PetController.owners</t>
+  </si>
+  <si>
+    <t>Has Field</t>
   </si>
 </sst>
 </file>
@@ -601,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,6 +1528,75 @@
         <v>5</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1501,9 +1605,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1834,6 +1940,48 @@
         <v>21</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1841,18 +1989,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2034,14 +2182,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2053,6 +2193,14 @@
     <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Se realiza la creación del stub
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prado\OneDrive\Documentos\GitHub\proyecto-grado\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC61DD4-7478-4623-A6E2-6D22932C3698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3A8B0-DF19-43A8-B94E-101AAAFDCD97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,9 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1989,6 +1987,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -2166,22 +2179,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2197,28 +2219,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se agregó el RestConfiguration y se corrigió JavaGeneratorMicroservices
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prado\OneDrive\Documentos\GitHub\proyecto-grado\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DC8B59-D87E-4DB2-A032-098FF8E610BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C14479C-22B9-4C53-8DF5-5F256EA8CA11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="103">
   <si>
     <t>Class</t>
   </si>
@@ -311,6 +311,36 @@
   </si>
   <si>
     <t>Microservice</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.boot.autoconfigure.SpringBootApplication</t>
+  </si>
+  <si>
+    <t>org.springframework.boot.autoconfigure</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>Has Annotation</t>
+  </si>
+  <si>
+    <t>pet1.org.springframework.boot.autoconfigure.SpringBootApplication</t>
+  </si>
+  <si>
+    <t>pet2.org.springframework.boot.autoconfigure.SpringBootApplication</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>Dst</t>
+  </si>
+  <si>
+    <t>owner.org.springframework.samples.petclinic.owner.OwnerRepository.save(Owner)</t>
+  </si>
+  <si>
+    <t>OwnerRepository.save(Owner)</t>
   </si>
 </sst>
 </file>
@@ -663,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1488,13 +1518,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
         <v>21</v>
@@ -1503,7 +1533,7 @@
         <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
@@ -1511,30 +1541,30 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
         <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
         <v>70</v>
@@ -1549,15 +1579,15 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
         <v>70</v>
@@ -1572,44 +1602,44 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="G39" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
         <v>32</v>
       </c>
       <c r="G40" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
         <v>21</v>
@@ -1626,7 +1656,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
@@ -1644,18 +1674,18 @@
         <v>32</v>
       </c>
       <c r="G42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
         <v>21</v>
@@ -1672,24 +1702,116 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
         <v>21</v>
       </c>
       <c r="E44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" t="s">
         <v>0</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>24</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1701,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:XFD32"/>
+  <dimension ref="A1:XFD39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,8 +1836,21 @@
     <col min="3" max="3" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1729,7 +1864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1743,7 +1878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1757,7 +1892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1771,7 +1906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1799,7 +1934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1813,7 +1948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1827,7 +1962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1841,7 +1976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1855,7 +1990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1869,7 +2004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -5978,7 +6113,7 @@
       <c r="XEZ13" s="1"/>
       <c r="XFD13" s="1"/>
     </row>
-    <row r="14" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -10087,7 +10222,7 @@
       <c r="XEZ14" s="1"/>
       <c r="XFD14" s="1"/>
     </row>
-    <row r="15" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -10101,7 +10236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -10115,7 +10250,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -10129,7 +10264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -10143,7 +10278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -10157,7 +10292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -10171,7 +10306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -10185,7 +10320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -10199,7 +10334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -10213,7 +10348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -10227,7 +10362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -10241,7 +10376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -10255,7 +10390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -10269,7 +10404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -10283,7 +10418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -10297,7 +10432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -10311,7 +10446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -10325,7 +10460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -10339,6 +10474,69 @@
         <v>21</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10346,21 +10544,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -10538,31 +10721,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10578,4 +10752,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se agrego las clases e configuracion de las entidades
</commit_message>
<xml_diff>
--- a/input/graph.xlsx
+++ b/input/graph.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prado\OneDrive\Documentos\GitHub\proyecto-grado\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelso\Documents\GitHub\proyecto-grado\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C14479C-22B9-4C53-8DF5-5F256EA8CA11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676A7975-4525-463B-87A3-7011510F6A52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -695,23 +695,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="96.21875" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" customWidth="1"/>
-    <col min="3" max="3" width="69.77734375" customWidth="1"/>
+    <col min="1" max="1" width="96.1796875" customWidth="1"/>
+    <col min="2" max="2" width="45.1796875" customWidth="1"/>
+    <col min="3" max="3" width="69.81640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="5" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -734,7 +734,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -757,7 +757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -780,7 +780,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -803,7 +803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -826,7 +826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -849,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -872,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -895,7 +895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -918,7 +918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -941,7 +941,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -964,7 +964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -987,7 +987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>101</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1823,20 +1823,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:XFD39"/>
+  <dimension ref="A1:XFD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="84.77734375" customWidth="1"/>
-    <col min="2" max="2" width="99.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="84.81640625" customWidth="1"/>
+    <col min="2" max="2" width="99.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -6113,7 +6113,7 @@
       <c r="XEZ13" s="1"/>
       <c r="XFD13" s="1"/>
     </row>
-    <row r="14" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -10222,7 +10222,7 @@
       <c r="XEZ14" s="1"/>
       <c r="XFD14" s="1"/>
     </row>
-    <row r="15" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -10278,7 +10278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -10334,7 +10334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -10362,7 +10362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -10418,7 +10418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -10474,7 +10474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -10488,7 +10488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -10502,7 +10502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -10530,13 +10530,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10544,6 +10543,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008352E896BEBC3B4BBE556B9821A22447" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f913282166a0f4e6fae5234b1a10d1bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a77fb7f8-12c9-4609-ac08-7d2a28f77de9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1fdcbb55615e8c28d62e918f83ed0de" ns2:_="">
     <xsd:import namespace="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
@@ -10721,22 +10735,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3839E01-B9A0-42A9-8974-3B924CEB6D59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10752,28 +10775,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D41A2B81-AB11-41E7-9B8C-6A9391946BF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4066899A-7741-4BF8-9BC2-E588D9B1CCA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a77fb7f8-12c9-4609-ac08-7d2a28f77de9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>